<commit_message>
fix NullPointerException if some data in file to be imported is not populated
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>John</t>
   </si>
@@ -38,18 +38,9 @@
     <t>Black</t>
   </si>
   <si>
-    <t>john@epam.com</t>
-  </si>
-  <si>
     <t>mary@epam.com</t>
   </si>
   <si>
-    <t>john@john.com</t>
-  </si>
-  <si>
-    <t>mary@mary.com</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -60,6 +51,12 @@
   </si>
   <si>
     <t>personal_email</t>
+  </si>
+  <si>
+    <t>john@personal.com</t>
+  </si>
+  <si>
+    <t>mary@personal.com</t>
   </si>
 </sst>
 </file>
@@ -377,62 +374,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapt to new file format
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -377,15 +377,15 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
@@ -397,7 +397,7 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -422,7 +422,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="I3" t="s">

</xml_diff>